<commit_message>
Manage Claims Email Update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="185">
   <si>
     <t>shipmentType</t>
   </si>
@@ -545,6 +545,45 @@
   </si>
   <si>
     <t>DropOff741</t>
+  </si>
+  <si>
+    <t>57794958</t>
+  </si>
+  <si>
+    <t>10-15-2021</t>
+  </si>
+  <si>
+    <t>$688.73</t>
+  </si>
+  <si>
+    <t>FCT898607587350544384</t>
+  </si>
+  <si>
+    <t>FCTEST1003764</t>
+  </si>
+  <si>
+    <t>$27.27</t>
+  </si>
+  <si>
+    <t>PickUp69</t>
+  </si>
+  <si>
+    <t>DropOff124</t>
+  </si>
+  <si>
+    <t>57794961</t>
+  </si>
+  <si>
+    <t>FCT898617792033456128</t>
+  </si>
+  <si>
+    <t>FCTEST1003765</t>
+  </si>
+  <si>
+    <t>PickUp90</t>
+  </si>
+  <si>
+    <t>DropOff660</t>
   </si>
 </sst>
 </file>
@@ -573,7 +612,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="126">
+  <fills count="198">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1200,8 +1239,368 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="124">
+  <borders count="196">
     <border>
       <left/>
       <right/>
@@ -1876,11 +2275,263 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="124">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1968,7 +2619,43 @@
     <xf applyBorder="true" applyFill="true" borderId="117" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="119" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="121" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="125" borderId="123" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="123" fillId="125" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="125" fillId="127" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="127" fillId="129" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="129" fillId="131" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="131" fillId="133" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="133" fillId="135" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="135" fillId="137" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="137" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="139" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="141" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="143" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="145" fillId="147" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="147" fillId="149" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="149" fillId="151" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="151" fillId="153" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="153" fillId="155" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="155" fillId="157" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="157" fillId="159" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="159" fillId="161" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="161" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="163" fillId="165" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="165" fillId="167" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="167" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="169" fillId="171" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="171" fillId="173" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="173" fillId="175" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="175" fillId="177" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="177" fillId="179" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="179" fillId="181" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="181" fillId="183" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="183" fillId="185" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="185" fillId="187" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="187" fillId="189" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="189" fillId="191" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="191" fillId="193" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="193" fillId="195" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="197" borderId="195" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2429,8 +3116,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="86" t="s">
-        <v>170</v>
+      <c r="C2" s="114" t="s">
+        <v>183</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -2453,8 +3140,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="87" t="s">
-        <v>171</v>
+      <c r="K2" s="115" t="s">
+        <v>184</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -2599,8 +3286,8 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="80" t="s">
-        <v>167</v>
+      <c r="B2" s="90" t="s">
+        <v>173</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -2651,31 +3338,31 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="U2" s="81" t="s">
-        <v>124</v>
+      <c r="T2" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="U2" s="91" t="s">
+        <v>174</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="82" t="s">
-        <v>168</v>
-      </c>
-      <c r="X2" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y2" s="84" t="s">
-        <v>125</v>
+      <c r="W2" s="92" t="s">
+        <v>175</v>
+      </c>
+      <c r="X2" s="93" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y2" s="94" t="s">
+        <v>177</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>150</v>
+      <c r="B3" s="108" t="s">
+        <v>173</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -2726,22 +3413,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="U3" s="63" t="s">
+      <c r="T3" s="107" t="s">
+        <v>180</v>
+      </c>
+      <c r="U3" s="109" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="X3" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y3" s="66"/>
+      <c r="W3" s="110" t="s">
+        <v>181</v>
+      </c>
+      <c r="X3" s="111" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y3" s="112"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2893,14 +3580,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="85" t="s">
-        <v>82</v>
+      <c r="A2" s="98" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
@@ -2937,13 +3624,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="71" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="77" t="s">
+      <c r="A3" s="116" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="117" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="123" t="s">
         <v>139</v>
       </c>
       <c r="D3" s="15" t="s">

</xml_diff>

<commit_message>
Separate suites for qa and stging and message update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="274">
   <si>
     <t>shipmentType</t>
   </si>
@@ -635,6 +635,222 @@
   </si>
   <si>
     <t>DropOff123</t>
+  </si>
+  <si>
+    <t>10-29-2021</t>
+  </si>
+  <si>
+    <t>Pending Tracking...</t>
+  </si>
+  <si>
+    <t>PickUp951</t>
+  </si>
+  <si>
+    <t>DropOff482</t>
+  </si>
+  <si>
+    <t>57905039</t>
+  </si>
+  <si>
+    <t>FCT903465593636651008</t>
+  </si>
+  <si>
+    <t>FCTEST1003836</t>
+  </si>
+  <si>
+    <t>PickUp918</t>
+  </si>
+  <si>
+    <t>DropOff908</t>
+  </si>
+  <si>
+    <t>57905041</t>
+  </si>
+  <si>
+    <t>FCT903478420304822272</t>
+  </si>
+  <si>
+    <t>FCTEST1003837</t>
+  </si>
+  <si>
+    <t>PickUp581</t>
+  </si>
+  <si>
+    <t>DropOff815</t>
+  </si>
+  <si>
+    <t>57905042</t>
+  </si>
+  <si>
+    <t>FCT903485001817915392</t>
+  </si>
+  <si>
+    <t>FCTEST1003838</t>
+  </si>
+  <si>
+    <t>PickUp637</t>
+  </si>
+  <si>
+    <t>DropOff954</t>
+  </si>
+  <si>
+    <t>57905047</t>
+  </si>
+  <si>
+    <t>FCT903502514618368000</t>
+  </si>
+  <si>
+    <t>FCTEST1003839</t>
+  </si>
+  <si>
+    <t>PickUp357</t>
+  </si>
+  <si>
+    <t>DropOff952</t>
+  </si>
+  <si>
+    <t>58138735</t>
+  </si>
+  <si>
+    <t>11-02-2021</t>
+  </si>
+  <si>
+    <t>FCT904983283735986176</t>
+  </si>
+  <si>
+    <t>FCTEST1003830</t>
+  </si>
+  <si>
+    <t>PickUp237</t>
+  </si>
+  <si>
+    <t>DropOff731</t>
+  </si>
+  <si>
+    <t>58138742</t>
+  </si>
+  <si>
+    <t>FCT904988968162951168</t>
+  </si>
+  <si>
+    <t>FCTEST1003831</t>
+  </si>
+  <si>
+    <t>PickUp318</t>
+  </si>
+  <si>
+    <t>DropOff353</t>
+  </si>
+  <si>
+    <t>58138775</t>
+  </si>
+  <si>
+    <t>FCT904996812262211584</t>
+  </si>
+  <si>
+    <t>FCTEST1003832</t>
+  </si>
+  <si>
+    <t>PickUp306</t>
+  </si>
+  <si>
+    <t>DropOff373</t>
+  </si>
+  <si>
+    <t>58138779</t>
+  </si>
+  <si>
+    <t>FCT905007525391237120</t>
+  </si>
+  <si>
+    <t>PickUp594</t>
+  </si>
+  <si>
+    <t>DropOff914</t>
+  </si>
+  <si>
+    <t>58138780</t>
+  </si>
+  <si>
+    <t>FCT905029865722347520</t>
+  </si>
+  <si>
+    <t>FCTEST1003834</t>
+  </si>
+  <si>
+    <t>PickUp15</t>
+  </si>
+  <si>
+    <t>DropOff305</t>
+  </si>
+  <si>
+    <t>58138784</t>
+  </si>
+  <si>
+    <t>FCT905043390154932224</t>
+  </si>
+  <si>
+    <t>FCTEST1003835</t>
+  </si>
+  <si>
+    <t>PickUp691</t>
+  </si>
+  <si>
+    <t>DropOff82</t>
+  </si>
+  <si>
+    <t>58138837</t>
+  </si>
+  <si>
+    <t>FCT905095710293098496</t>
+  </si>
+  <si>
+    <t>PickUp366</t>
+  </si>
+  <si>
+    <t>DropOff454</t>
+  </si>
+  <si>
+    <t>58138838</t>
+  </si>
+  <si>
+    <t>FCT905161152848199680</t>
+  </si>
+  <si>
+    <t>PickUp561</t>
+  </si>
+  <si>
+    <t>DropOff937</t>
+  </si>
+  <si>
+    <t>11-03-2021</t>
+  </si>
+  <si>
+    <t>58193236</t>
+  </si>
+  <si>
+    <t>11-08-2021</t>
+  </si>
+  <si>
+    <t>FCT907201162267066368</t>
+  </si>
+  <si>
+    <t>PickUp310</t>
+  </si>
+  <si>
+    <t>DropOff18</t>
+  </si>
+  <si>
+    <t>58193243</t>
+  </si>
+  <si>
+    <t>FCT907212077263749120</t>
+  </si>
+  <si>
+    <t>PickUp203</t>
+  </si>
+  <si>
+    <t>DropOff753</t>
   </si>
 </sst>
 </file>
@@ -663,7 +879,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="306">
+  <fills count="788">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2190,8 +2406,2418 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="304">
+  <borders count="786">
     <border>
       <left/>
       <right/>
@@ -3496,11 +6122,1698 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="419">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -3678,7 +7991,248 @@
     <xf applyBorder="true" applyFill="true" borderId="297" fillId="299" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="299" fillId="301" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="301" fillId="303" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="305" borderId="303" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="303" fillId="305" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="305" fillId="307" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="307" fillId="309" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="309" fillId="311" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="311" fillId="313" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="313" fillId="315" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="315" fillId="317" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="317" fillId="319" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="319" fillId="321" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="321" fillId="323" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="323" fillId="325" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="325" fillId="327" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="327" fillId="329" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="329" fillId="331" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="331" fillId="333" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="333" fillId="335" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="335" fillId="337" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="337" fillId="339" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="339" fillId="341" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="341" fillId="343" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="343" fillId="345" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="345" fillId="347" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="347" fillId="349" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="349" fillId="351" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="351" fillId="353" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="353" fillId="355" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="355" fillId="357" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="357" fillId="359" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="359" fillId="361" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="361" fillId="363" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="363" fillId="365" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="365" fillId="367" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="367" fillId="369" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="369" fillId="371" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="371" fillId="373" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="373" fillId="375" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="375" fillId="377" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="377" fillId="379" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="379" fillId="381" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="381" fillId="383" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="383" fillId="385" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="385" fillId="387" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="387" fillId="389" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="389" fillId="391" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="391" fillId="393" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="393" fillId="395" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="395" fillId="397" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="397" fillId="399" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="399" fillId="401" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="401" fillId="403" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="403" fillId="405" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="405" fillId="407" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="407" fillId="409" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="409" fillId="411" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="411" fillId="413" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="413" fillId="415" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="415" fillId="417" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="417" fillId="419" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="419" fillId="421" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="421" fillId="423" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="423" fillId="425" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="425" fillId="427" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="427" fillId="429" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="429" fillId="431" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="431" fillId="433" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="433" fillId="435" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="435" fillId="437" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="437" fillId="439" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="439" fillId="441" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="441" fillId="443" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="443" fillId="445" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="445" fillId="447" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="447" fillId="449" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="449" fillId="451" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="451" fillId="453" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="453" fillId="455" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="455" fillId="457" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="457" fillId="459" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="459" fillId="461" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="461" fillId="463" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="463" fillId="465" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="465" fillId="467" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="467" fillId="469" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="469" fillId="471" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="471" fillId="473" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="473" fillId="475" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="475" fillId="477" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="477" fillId="479" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="479" fillId="481" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="481" fillId="483" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="483" fillId="485" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="485" fillId="487" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="487" fillId="489" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="489" fillId="491" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="491" fillId="493" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="493" fillId="495" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="495" fillId="497" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="497" fillId="499" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="499" fillId="501" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="501" fillId="503" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="503" fillId="505" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="505" fillId="507" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="507" fillId="509" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="509" fillId="511" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="511" fillId="513" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="513" fillId="515" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="515" fillId="517" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="517" fillId="519" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="519" fillId="521" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="521" fillId="523" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="523" fillId="525" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="525" fillId="527" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="527" fillId="529" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="529" fillId="531" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="531" fillId="533" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="533" fillId="535" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="535" fillId="537" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="537" fillId="539" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="539" fillId="541" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="541" fillId="543" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="543" fillId="545" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="545" fillId="547" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="547" fillId="549" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="549" fillId="551" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="551" fillId="553" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="553" fillId="555" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="555" fillId="557" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="557" fillId="559" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="559" fillId="561" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="561" fillId="563" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="563" fillId="565" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="565" fillId="567" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="567" fillId="569" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="569" fillId="571" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="571" fillId="573" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="573" fillId="575" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="575" fillId="577" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="577" fillId="579" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="579" fillId="581" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="581" fillId="583" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="583" fillId="585" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="585" fillId="587" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="587" fillId="589" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="589" fillId="591" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="591" fillId="593" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="593" fillId="595" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="595" fillId="597" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="597" fillId="599" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="599" fillId="601" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="601" fillId="603" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="603" fillId="605" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="605" fillId="607" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="607" fillId="609" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="609" fillId="611" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="611" fillId="613" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="613" fillId="615" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="615" fillId="617" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="617" fillId="619" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="619" fillId="621" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="621" fillId="623" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="623" fillId="625" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="625" fillId="627" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="627" fillId="629" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="629" fillId="631" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="631" fillId="633" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="633" fillId="635" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="635" fillId="637" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="637" fillId="639" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="639" fillId="641" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="641" fillId="643" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="643" fillId="645" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="645" fillId="647" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="647" fillId="649" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="649" fillId="651" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="651" fillId="653" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="653" fillId="655" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="655" fillId="657" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="657" fillId="659" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="659" fillId="661" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="661" fillId="663" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="663" fillId="665" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="665" fillId="667" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="667" fillId="669" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="669" fillId="671" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="671" fillId="673" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="673" fillId="675" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="675" fillId="677" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="677" fillId="679" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="679" fillId="681" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="681" fillId="683" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="683" fillId="685" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="685" fillId="687" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="687" fillId="689" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="689" fillId="691" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="691" fillId="693" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="693" fillId="695" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="695" fillId="697" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="697" fillId="699" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="699" fillId="701" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="701" fillId="703" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="703" fillId="705" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="705" fillId="707" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="707" fillId="709" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="709" fillId="711" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="711" fillId="713" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="713" fillId="715" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="715" fillId="717" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="717" fillId="719" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="719" fillId="721" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="721" fillId="723" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="723" fillId="725" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="725" fillId="727" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="727" fillId="729" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="729" fillId="731" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="731" fillId="733" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="733" fillId="735" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="735" fillId="737" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="737" fillId="739" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="739" fillId="741" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="741" fillId="743" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="743" fillId="745" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="745" fillId="747" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="747" fillId="749" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="749" fillId="751" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="751" fillId="753" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="753" fillId="755" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="755" fillId="757" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="757" fillId="759" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="759" fillId="761" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="761" fillId="763" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="763" fillId="765" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="765" fillId="767" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="767" fillId="769" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="769" fillId="771" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="771" fillId="773" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="773" fillId="775" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="775" fillId="777" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="777" fillId="779" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="779" fillId="781" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="781" fillId="783" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="783" fillId="785" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="787" borderId="785" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4139,8 +8693,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="176" t="s">
-        <v>200</v>
+      <c r="C2" s="409" t="s">
+        <v>272</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -4163,8 +8717,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="177" t="s">
-        <v>201</v>
+      <c r="K2" s="410" t="s">
+        <v>273</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -4309,8 +8863,8 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="170" t="s">
-        <v>197</v>
+      <c r="B2" s="385" t="s">
+        <v>266</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -4361,22 +8915,22 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="169" t="s">
-        <v>196</v>
-      </c>
-      <c r="U2" s="171" t="s">
+      <c r="T2" s="384" t="s">
+        <v>265</v>
+      </c>
+      <c r="U2" s="386" t="s">
         <v>174</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="172" t="s">
-        <v>198</v>
-      </c>
-      <c r="X2" s="173" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y2" s="174" t="s">
+      <c r="W2" s="387" t="s">
+        <v>267</v>
+      </c>
+      <c r="X2" s="388" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y2" s="389" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4384,8 +8938,8 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="149" t="s">
-        <v>185</v>
+      <c r="B3" s="403" t="s">
+        <v>266</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -4436,22 +8990,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="148" t="s">
-        <v>191</v>
-      </c>
-      <c r="U3" s="150" t="s">
+      <c r="T3" s="402" t="s">
+        <v>270</v>
+      </c>
+      <c r="U3" s="404" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="151" t="s">
-        <v>192</v>
-      </c>
-      <c r="X3" s="152" t="s">
-        <v>193</v>
-      </c>
-      <c r="Y3" s="153"/>
+      <c r="W3" s="405" t="s">
+        <v>271</v>
+      </c>
+      <c r="X3" s="406" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y3" s="407"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4603,14 +9157,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="140" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="175" t="s">
-        <v>82</v>
+      <c r="A2" s="393" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="394" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="400" t="s">
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
@@ -4647,13 +9201,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" s="117" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="162" t="s">
+      <c r="A3" s="411" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="412" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="418" t="s">
         <v>139</v>
       </c>
       <c r="D3" s="15" t="s">

</xml_diff>

<commit_message>
Uncomment BOL, Labels and ZPL
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="274">
   <si>
     <t>shipmentType</t>
   </si>
@@ -879,7 +879,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="788">
+  <fills count="792">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4816,8 +4816,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="786">
+  <borders count="790">
     <border>
       <left/>
       <right/>
@@ -7809,11 +7829,25 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="419">
+  <cellXfs count="421">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -8232,7 +8266,9 @@
     <xf applyBorder="true" applyFill="true" borderId="779" fillId="781" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="781" fillId="783" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="783" fillId="785" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="787" borderId="785" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="785" fillId="787" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="787" fillId="789" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="791" borderId="789" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -8915,8 +8951,8 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="384" t="s">
-        <v>265</v>
+      <c r="T2" s="420" t="s">
+        <v>79</v>
       </c>
       <c r="U2" s="386" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
Test and bat update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1F1DB8-087F-4954-9BCA-9422C7C48020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2D1F1DB8-087F-4954-9BCA-9422C7C48020}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="669" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="2" tabRatio="669" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateAccount" sheetId="5" r:id="rId1"/>
-    <sheet name="ShipmentInformation" sheetId="6" r:id="rId2"/>
-    <sheet name="Input" sheetId="1" r:id="rId3"/>
-    <sheet name="ClaimDetail" sheetId="7" r:id="rId4"/>
-    <sheet name="ContactInfo" sheetId="8" r:id="rId5"/>
+    <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
+    <sheet name="ShipmentInformation" r:id="rId2" sheetId="6"/>
+    <sheet name="Input" r:id="rId3" sheetId="1"/>
+    <sheet name="ClaimDetail" r:id="rId4" sheetId="7"/>
+    <sheet name="ContactInfo" r:id="rId5" sheetId="8"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="166">
   <si>
     <t>shipmentType</t>
   </si>
@@ -479,12 +479,61 @@
   </si>
   <si>
     <t>DropOff100</t>
+  </si>
+  <si>
+    <t>58233442</t>
+  </si>
+  <si>
+    <t>11-18-2021</t>
+  </si>
+  <si>
+    <t>FCT910922194140266496</t>
+  </si>
+  <si>
+    <t>FCTEST1003955</t>
+  </si>
+  <si>
+    <t>PickUp682</t>
+  </si>
+  <si>
+    <t>DropOff534</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Filed - Additional Docs Needed</t>
+  </si>
+  <si>
+    <t>Filed - Review</t>
+  </si>
+  <si>
+    <t>Pending Documentation</t>
+  </si>
+  <si>
+    <t>58233443</t>
+  </si>
+  <si>
+    <t>$673.02</t>
+  </si>
+  <si>
+    <t>FCT910932700171337728</t>
+  </si>
+  <si>
+    <t>FCTEST1003956</t>
+  </si>
+  <si>
+    <t>PickUp79</t>
+  </si>
+  <si>
+    <t>DropOff698</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,7 +555,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="106">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,8 +722,368 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="104">
     <border>
       <left/>
       <right/>
@@ -1027,59 +1436,347 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+  <cellXfs count="78">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="6" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="7" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="8" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="9" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="10" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="10" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="11" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="12" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="13" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="16" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="17" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="18" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="19" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="20" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="21" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="22" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="23" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="24" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="25" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="26" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="27" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="28" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="29" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="30" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="31" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="33" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="35" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="37" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="47" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="49" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="51" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="53" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="55" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="57" fillId="59" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="59" fillId="61" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="61" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="63" fillId="65" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="65" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="67" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="69" fillId="71" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="71" fillId="73" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="73" fillId="75" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="75" fillId="77" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="77" fillId="79" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="79" fillId="81" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="81" fillId="83" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="83" fillId="85" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="85" fillId="87" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="87" fillId="89" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="89" fillId="91" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="91" fillId="93" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="93" fillId="95" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="95" fillId="97" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="97" fillId="99" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="99" fillId="101" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="101" fillId="103" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="105" borderId="103" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1096,10 +1793,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1263,21 +1960,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1294,7 +1991,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1346,15 +2043,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1362,15 +2059,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="7" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="7" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" style="7" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1432,14 +2129,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
@@ -1447,28 +2144,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.38671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.25" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1534,8 +2231,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>148</v>
+      <c r="C2" s="68" t="s">
+        <v>164</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -1558,8 +2255,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="39" t="s">
-        <v>149</v>
+      <c r="K2" s="69" t="s">
+        <v>165</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -1584,14 +2281,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
@@ -1599,28 +2296,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="33.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="14" width="9.140625" style="1" collapsed="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.140625" style="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.140625" style="1" collapsed="1"/>
-    <col min="20" max="20" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="24.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.43359375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="31.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" style="1" width="33.42578125" collapsed="true"/>
+    <col min="12" max="14" style="1" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="16" max="16" style="1" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="19" style="1" width="9.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.95703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.28125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="24.36328125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="15.25390625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="9.76171875" collapsed="true"/>
+    <col min="26" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -1700,12 +2397,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15.75" r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>144</v>
+      <c r="B2" s="44" t="s">
+        <v>151</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -1756,31 +2453,31 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="33" t="s">
+      <c r="T2" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="U2" s="45" t="s">
         <v>145</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="X2" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y2" s="36" t="s">
+      <c r="W2" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="X2" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y2" s="48" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15.75" r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>141</v>
+      <c r="B3" s="62" t="s">
+        <v>151</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -1831,24 +2528,24 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>138</v>
+      <c r="T3" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="U3" s="63" t="s">
+        <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="X3" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y3" s="28"/>
+      <c r="W3" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="X3" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y3" s="66"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>85</v>
       </c>
@@ -1914,14 +2611,14 @@
       <c r="Y4" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753CECDE-5C6C-44FA-B81E-EDD6D441D136}">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753CECDE-5C6C-44FA-B81E-EDD6D441D136}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -1929,22 +2626,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="59.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.3046875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5859375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="59.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1998,14 +2695,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>82</v>
+      <c r="A2" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
@@ -2042,13 +2739,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="77" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -2129,14 +2826,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81E9B93-CAE0-4779-9186-88D86220B35C}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81E9B93-CAE0-4779-9186-88D86220B35C}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -2144,11 +2841,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2171,7 +2868,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>101</v>
       </c>
@@ -2210,9 +2907,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{BB1CBF5B-2715-4060-9476-DC733E28C200}"/>
+    <hyperlink r:id="rId1" ref="E2" xr:uid="{BB1CBF5B-2715-4060-9476-DC733E28C200}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Manage Invoice fix - 3rd time
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
   <si>
     <t>shipmentType</t>
   </si>
@@ -527,6 +527,24 @@
   </si>
   <si>
     <t>DropOff698</t>
+  </si>
+  <si>
+    <t>58285545</t>
+  </si>
+  <si>
+    <t>11-25-2021</t>
+  </si>
+  <si>
+    <t>FCT913424965259231232</t>
+  </si>
+  <si>
+    <t>FCTEST1003996</t>
+  </si>
+  <si>
+    <t>PickUp607</t>
+  </si>
+  <si>
+    <t>DropOff193</t>
   </si>
 </sst>
 </file>
@@ -555,7 +573,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="106">
+  <fills count="126">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1082,8 +1100,108 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="104">
+  <borders count="124">
     <border>
       <left/>
       <right/>
@@ -1688,11 +1806,81 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1770,7 +1958,17 @@
     <xf applyBorder="true" applyFill="true" borderId="97" fillId="99" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="99" fillId="101" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="101" fillId="103" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="105" borderId="103" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="103" fillId="105" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="105" fillId="107" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="107" fillId="109" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="109" fillId="111" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="111" fillId="113" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="113" fillId="115" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="115" fillId="117" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="117" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="119" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="121" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="125" borderId="123" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2231,8 +2429,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="68" t="s">
-        <v>164</v>
+      <c r="C2" s="86" t="s">
+        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -2255,8 +2453,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="69" t="s">
-        <v>165</v>
+      <c r="K2" s="87" t="s">
+        <v>171</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -2476,8 +2674,8 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>151</v>
+      <c r="B3" s="80" t="s">
+        <v>167</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -2528,22 +2726,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="U3" s="63" t="s">
+      <c r="T3" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="U3" s="81" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="X3" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y3" s="66"/>
+      <c r="W3" s="82" t="s">
+        <v>168</v>
+      </c>
+      <c r="X3" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y3" s="84"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2745,8 +2943,8 @@
       <c r="B3" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="77" t="s">
-        <v>137</v>
+      <c r="C3" s="85" t="s">
+        <v>82</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Manage Invoice fix - 4th time
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
   <si>
     <t>shipmentType</t>
   </si>
@@ -545,6 +545,21 @@
   </si>
   <si>
     <t>DropOff193</t>
+  </si>
+  <si>
+    <t>58285547</t>
+  </si>
+  <si>
+    <t>FCT913438719413846016</t>
+  </si>
+  <si>
+    <t>FCTEST1003998</t>
+  </si>
+  <si>
+    <t>PickUp174</t>
+  </si>
+  <si>
+    <t>DropOff53</t>
   </si>
 </sst>
 </file>
@@ -573,7 +588,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="126">
+  <fills count="146">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1200,8 +1215,108 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="124">
+  <borders count="144">
     <border>
       <left/>
       <right/>
@@ -1876,11 +1991,81 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1968,7 +2153,17 @@
     <xf applyBorder="true" applyFill="true" borderId="117" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="119" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="121" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="125" borderId="123" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="123" fillId="125" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="125" fillId="127" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="127" fillId="129" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="129" fillId="131" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="131" fillId="133" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="133" fillId="135" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="135" fillId="137" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="137" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="139" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="141" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="145" borderId="143" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2429,8 +2624,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="86" t="s">
-        <v>170</v>
+      <c r="C2" s="96" t="s">
+        <v>175</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -2453,8 +2648,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="87" t="s">
-        <v>171</v>
+      <c r="K2" s="97" t="s">
+        <v>176</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -2674,7 +2869,7 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="90" t="s">
         <v>167</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2726,22 +2921,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="U3" s="81" t="s">
+      <c r="T3" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="U3" s="91" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="82" t="s">
-        <v>168</v>
-      </c>
-      <c r="X3" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y3" s="84"/>
+      <c r="W3" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="X3" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y3" s="94"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2943,7 +3138,7 @@
       <c r="B3" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="95" t="s">
         <v>82</v>
       </c>
       <c r="D3" s="15" t="s">

</xml_diff>

<commit_message>
qq and custom suite update
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageClaims.xlsx
+++ b/binaries/FCfiles/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="193">
   <si>
     <t>shipmentType</t>
   </si>
@@ -560,6 +560,54 @@
   </si>
   <si>
     <t>DropOff53</t>
+  </si>
+  <si>
+    <t>58327782</t>
+  </si>
+  <si>
+    <t>12-01-2021</t>
+  </si>
+  <si>
+    <t>FCT915497466927775744</t>
+  </si>
+  <si>
+    <t>FCTEST1004007</t>
+  </si>
+  <si>
+    <t>PickUp674</t>
+  </si>
+  <si>
+    <t>DropOff363</t>
+  </si>
+  <si>
+    <t>58327789</t>
+  </si>
+  <si>
+    <t>FCT915506118178897920</t>
+  </si>
+  <si>
+    <t>FCTEST1004009</t>
+  </si>
+  <si>
+    <t>PickUp123</t>
+  </si>
+  <si>
+    <t>DropOff843</t>
+  </si>
+  <si>
+    <t>58327790</t>
+  </si>
+  <si>
+    <t>FCT915518758829686784</t>
+  </si>
+  <si>
+    <t>FCTEST1004010</t>
+  </si>
+  <si>
+    <t>PickUp15</t>
+  </si>
+  <si>
+    <t>DropOff445</t>
   </si>
 </sst>
 </file>
@@ -588,7 +636,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="146">
+  <fills count="232">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1315,8 +1363,438 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="144">
+  <borders count="230">
     <border>
       <left/>
       <right/>
@@ -2061,11 +2539,312 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="141">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -2163,7 +2942,50 @@
     <xf applyBorder="true" applyFill="true" borderId="137" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="139" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="141" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="145" borderId="143" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="143" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="145" fillId="147" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="147" fillId="149" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="149" fillId="151" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="151" fillId="153" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="153" fillId="155" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="155" fillId="157" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="157" fillId="159" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="159" fillId="161" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="161" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="163" fillId="165" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="165" fillId="167" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="167" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="169" fillId="171" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="171" fillId="173" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="173" fillId="175" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="175" fillId="177" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="177" fillId="179" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="179" fillId="181" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="181" fillId="183" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="183" fillId="185" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="185" fillId="187" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="187" fillId="189" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="189" fillId="191" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="191" fillId="193" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="193" fillId="195" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="195" fillId="197" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="197" fillId="199" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="199" fillId="201" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="201" fillId="203" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="203" fillId="205" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="205" fillId="207" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="207" fillId="209" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="209" fillId="211" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="211" fillId="213" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="213" fillId="215" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="215" fillId="217" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="217" fillId="219" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="219" fillId="221" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="221" fillId="223" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="223" fillId="225" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="225" fillId="227" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="227" fillId="229" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="231" borderId="229" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2624,8 +3446,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="96" t="s">
-        <v>175</v>
+      <c r="C2" s="133" t="s">
+        <v>191</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -2648,8 +3470,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="97" t="s">
-        <v>176</v>
+      <c r="K2" s="134" t="s">
+        <v>192</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -2794,8 +3616,8 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>151</v>
+      <c r="B2" s="111" t="s">
+        <v>178</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -2846,22 +3668,22 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="45" t="s">
+      <c r="T2" s="110" t="s">
+        <v>183</v>
+      </c>
+      <c r="U2" s="112" t="s">
         <v>145</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="X2" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y2" s="48" t="s">
+      <c r="W2" s="113" t="s">
+        <v>184</v>
+      </c>
+      <c r="X2" s="114" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y2" s="115" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2869,8 +3691,8 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="90" t="s">
-        <v>167</v>
+      <c r="B3" s="127" t="s">
+        <v>178</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -2921,22 +3743,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="89" t="s">
-        <v>172</v>
-      </c>
-      <c r="U3" s="91" t="s">
+      <c r="T3" s="126" t="s">
+        <v>188</v>
+      </c>
+      <c r="U3" s="128" t="s">
         <v>161</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W3" s="92" t="s">
-        <v>173</v>
-      </c>
-      <c r="X3" s="93" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y3" s="94"/>
+      <c r="W3" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="X3" s="130" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y3" s="131"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -3094,7 +3916,7 @@
       <c r="B2" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="124" t="s">
         <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3138,8 +3960,8 @@
       <c r="B3" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="95" t="s">
-        <v>82</v>
+      <c r="C3" s="140" t="s">
+        <v>137</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>81</v>

</xml_diff>